<commit_message>
link text added to the constact page
</commit_message>
<xml_diff>
--- a/docs/audit/audit-SEO.xlsx
+++ b/docs/audit/audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amama\Desktop\my projects\MahirAbubakar_P4_270621\docs\audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6D762F-C7F3-4398-A07F-006989B5F6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AAF1E6-BB91-4DD0-8246-ABCD69BD72A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="161">
   <si>
     <t>Catégorie</t>
   </si>
@@ -356,9 +356,6 @@
     <t>W3C Html&amp;Css</t>
   </si>
   <si>
-    <t>Test de crawlabilité sur Seolyser</t>
-  </si>
-  <si>
     <t>Test de vitesse sur Gtmetrix</t>
   </si>
   <si>
@@ -510,20 +507,41 @@
     <t>4. Analyser les liens</t>
   </si>
   <si>
-    <t>Existe-t-il des comptes sur les RS ?</t>
-  </si>
-  <si>
     <t>Présence des méta tag OG &amp; card twitter dans le code ?</t>
   </si>
   <si>
     <t>Présence de liens spammy ?</t>
+  </si>
+  <si>
+    <t>Adjacent links go to the same URL.</t>
+  </si>
+  <si>
+    <t>Very low contrast between text and background colors.</t>
+  </si>
+  <si>
+    <t>Adequate contrast of text is necessary for all users, especially users with low vision.</t>
+  </si>
+  <si>
+    <t>Increase the contrast between the foreground (text) color and the background color. Large text (larger than 18 point or 14 point bold) does not require as much contrast as smaller text.</t>
+  </si>
+  <si>
+    <t>Empty link</t>
+  </si>
+  <si>
+    <t>A link contains no text.</t>
+  </si>
+  <si>
+    <t>If a link contains no text, the function or purpose of the link will not be presented to the user. This can introduce confusion for keyboard and screen reader users.</t>
+  </si>
+  <si>
+    <t>Remove the empty link or provide text within the link that describes the functionality and/or target of that link.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -618,6 +636,36 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF444444"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF444444"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1451A0"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -842,7 +890,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -932,7 +980,6 @@
     <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -943,6 +990,15 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1227,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z950"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1318,7 +1374,7 @@
       <c r="E3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="82" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1729,13 +1785,58 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="B25" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="78" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="79" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="76" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" s="77" t="s">
+        <v>156</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B28" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="78" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" s="78" t="s">
+        <v>159</v>
+      </c>
+      <c r="E28" s="78" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2682,19 +2783,21 @@
     <hyperlink ref="F22" r:id="rId20" xr:uid="{14B53ED6-846B-4E81-9D64-51B89D68F26D}"/>
     <hyperlink ref="F3" r:id="rId21" xr:uid="{C127AC90-7988-4894-8707-37C29BA1ED14}"/>
     <hyperlink ref="F23" r:id="rId22" xr:uid="{4183097E-EC97-4711-8A44-3DBD94152F1C}"/>
+    <hyperlink ref="F27" r:id="rId23" location="sc1.4.3" xr:uid="{F1C69505-3DD6-42EF-A020-AE1E987F4078}"/>
+    <hyperlink ref="F28" r:id="rId24" location="sc1.4.3" xr:uid="{F23B87A4-0FB2-4BB0-ABB7-A11ABA15C8CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId23"/>
-  <drawing r:id="rId24"/>
+  <pageSetup orientation="landscape" r:id="rId25"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE5A153-4088-4B3A-B952-ECA3228BDD93}">
-  <dimension ref="A1:K84"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2705,14 +2808,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="76"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="75"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
@@ -2760,77 +2863,85 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+      <c r="B13" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
       <c r="B14" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="15"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="16" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B17" s="15"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="18"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="21"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="24"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="19"/>
-      <c r="B21" s="25" t="s">
-        <v>113</v>
-      </c>
+      <c r="A21" s="20"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -2855,38 +2966,38 @@
       <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="20"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="21"/>
+      <c r="A23" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="19"/>
+      <c r="B24" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="24"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="21"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="19"/>
-      <c r="B25" s="25" t="s">
-        <v>115</v>
-      </c>
+      <c r="A25" s="20"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -2898,36 +3009,38 @@
       <c r="K25" s="21"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="20"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
+      <c r="A26" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="24"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="19"/>
+      <c r="B27" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="24"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="21"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="19"/>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="26" t="s">
         <v>117</v>
       </c>
       <c r="C28" s="20"/>
@@ -2957,9 +3070,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="19"/>
-      <c r="B30" s="26" t="s">
-        <v>119</v>
-      </c>
+      <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
@@ -2971,109 +3082,109 @@
       <c r="K30" s="21"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="21"/>
+      <c r="A31" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="24"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="19"/>
+      <c r="B32" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="24"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="21"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="19"/>
-      <c r="B33" s="25" t="s">
+      <c r="A33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="29"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="21"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="29"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="32"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="33"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="35"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="32"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="33"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="35"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="24"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="34"/>
+      <c r="B38" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="24"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
+      <c r="K38" s="35"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="34"/>
-      <c r="B39" s="38" t="s">
-        <v>124</v>
-      </c>
+      <c r="B39" s="34"/>
       <c r="C39" s="34"/>
       <c r="D39" s="34"/>
       <c r="E39" s="34"/>
@@ -3085,94 +3196,94 @@
       <c r="K39" s="35"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
-      <c r="K40" s="35"/>
+      <c r="A40" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="24"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="34"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="35"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A42" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="24"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="34"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
-      <c r="K42" s="35"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="24"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
+      <c r="K43" s="35"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="37"/>
-      <c r="K43" s="24"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
-      <c r="K44" s="35"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="24"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="34"/>
+      <c r="B45" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="24"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="35"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="34"/>
-      <c r="B46" s="39" t="s">
-        <v>128</v>
-      </c>
+      <c r="B46" s="38"/>
       <c r="C46" s="34"/>
       <c r="D46" s="34"/>
       <c r="E46" s="34"/>
@@ -3184,60 +3295,62 @@
       <c r="K46" s="35"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" s="34"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="34"/>
-      <c r="K47" s="35"/>
+      <c r="A47" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="24"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="35"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A49" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="24"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="34"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34"/>
-      <c r="K49" s="35"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="24"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="34"/>
+      <c r="B50" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="37"/>
-      <c r="J50" s="37"/>
-      <c r="K50" s="24"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="35"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="34"/>
@@ -3255,34 +3368,34 @@
       <c r="K51" s="35"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52" s="34"/>
-      <c r="B52" s="39" t="s">
+      <c r="A52" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="34"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="34"/>
-      <c r="K52" s="35"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="24"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A53" s="40" t="s">
+      <c r="A53" s="42"/>
+      <c r="B53" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="B53" s="41"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="24"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="35"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="42"/>
@@ -3300,10 +3413,8 @@
       <c r="K54" s="35"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A55" s="42"/>
-      <c r="B55" s="39" t="s">
-        <v>135</v>
-      </c>
+      <c r="A55" s="34"/>
+      <c r="B55" s="39"/>
       <c r="C55" s="34"/>
       <c r="D55" s="34"/>
       <c r="E55" s="34"/>
@@ -3315,32 +3426,34 @@
       <c r="K55" s="35"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A56" s="34"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
-      <c r="H56" s="34"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="34"/>
-      <c r="K56" s="35"/>
+      <c r="A56" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="24"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A57" s="36" t="s">
+      <c r="A57" s="34"/>
+      <c r="B57" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="37"/>
-      <c r="K57" s="24"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="34"/>
+      <c r="K57" s="35"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="34"/>
@@ -3359,7 +3472,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="34"/>
-      <c r="B59" s="38" t="s">
+      <c r="B59" s="39" t="s">
         <v>138</v>
       </c>
       <c r="C59" s="34"/>
@@ -3374,9 +3487,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="34"/>
-      <c r="B60" s="39" t="s">
-        <v>139</v>
-      </c>
+      <c r="B60" s="38"/>
       <c r="C60" s="34"/>
       <c r="D60" s="34"/>
       <c r="E60" s="34"/>
@@ -3388,109 +3499,109 @@
       <c r="K60" s="35"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A61" s="34"/>
-      <c r="B61" s="38"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="34"/>
-      <c r="H61" s="34"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="34"/>
-      <c r="K61" s="35"/>
+      <c r="A61" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
+      <c r="K61" s="24"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A62" s="43" t="s">
+      <c r="A62" s="44"/>
+      <c r="B62" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="37"/>
-      <c r="I62" s="37"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="24"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+      <c r="H62" s="31"/>
+      <c r="I62" s="31"/>
+      <c r="J62" s="31"/>
+      <c r="K62" s="32"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A63" s="44"/>
-      <c r="B63" s="45" t="s">
+      <c r="A63" s="46"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="34"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="34"/>
+      <c r="J63" s="34"/>
+      <c r="K63" s="35"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A64" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31"/>
-      <c r="H63" s="31"/>
-      <c r="I63" s="31"/>
-      <c r="J63" s="31"/>
-      <c r="K63" s="32"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A64" s="46"/>
-      <c r="B64" s="39"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="34"/>
-      <c r="H64" s="34"/>
-      <c r="I64" s="34"/>
-      <c r="J64" s="34"/>
-      <c r="K64" s="35"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="49"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="49"/>
+      <c r="J64" s="49"/>
+      <c r="K64" s="24"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A65" s="47" t="s">
+      <c r="A65" s="50"/>
+      <c r="B65" s="51"/>
+      <c r="C65" s="52"/>
+      <c r="D65" s="52"/>
+      <c r="E65" s="52"/>
+      <c r="F65" s="52"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="52"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="53"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A67" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="B65" s="48"/>
-      <c r="C65" s="49"/>
-      <c r="D65" s="49"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="49"/>
-      <c r="G65" s="49"/>
-      <c r="H65" s="49"/>
-      <c r="I65" s="49"/>
-      <c r="J65" s="49"/>
-      <c r="K65" s="24"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A66" s="50"/>
-      <c r="B66" s="51"/>
-      <c r="C66" s="52"/>
-      <c r="D66" s="52"/>
-      <c r="E66" s="52"/>
-      <c r="F66" s="52"/>
-      <c r="G66" s="52"/>
-      <c r="H66" s="52"/>
-      <c r="I66" s="52"/>
-      <c r="J66" s="52"/>
-      <c r="K66" s="53"/>
+      <c r="B67" s="55"/>
+      <c r="C67" s="55"/>
+      <c r="D67" s="55"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="55"/>
+      <c r="G67" s="55"/>
+      <c r="H67" s="55"/>
+      <c r="I67" s="55"/>
+      <c r="J67" s="55"/>
+      <c r="K67" s="56"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A68" s="54" t="s">
+      <c r="A68" s="57"/>
+      <c r="B68" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="B68" s="55"/>
-      <c r="C68" s="55"/>
-      <c r="D68" s="55"/>
-      <c r="E68" s="55"/>
-      <c r="F68" s="55"/>
-      <c r="G68" s="55"/>
-      <c r="H68" s="55"/>
-      <c r="I68" s="55"/>
-      <c r="J68" s="55"/>
-      <c r="K68" s="56"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="59"/>
+      <c r="E68" s="59"/>
+      <c r="F68" s="59"/>
+      <c r="G68" s="59"/>
+      <c r="H68" s="59"/>
+      <c r="I68" s="59"/>
+      <c r="J68" s="59"/>
+      <c r="K68" s="60"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="57"/>
-      <c r="B69" s="58" t="s">
-        <v>144</v>
-      </c>
+      <c r="B69" s="58"/>
       <c r="C69" s="59"/>
       <c r="D69" s="59"/>
       <c r="E69" s="59"/>
@@ -3503,7 +3614,9 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="57"/>
-      <c r="B70" s="58"/>
+      <c r="B70" s="58" t="s">
+        <v>144</v>
+      </c>
       <c r="C70" s="59"/>
       <c r="D70" s="59"/>
       <c r="E70" s="59"/>
@@ -3531,9 +3644,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="57"/>
-      <c r="B72" s="58" t="s">
-        <v>146</v>
-      </c>
+      <c r="B72" s="58"/>
       <c r="C72" s="59"/>
       <c r="D72" s="59"/>
       <c r="E72" s="59"/>
@@ -3546,7 +3657,9 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="57"/>
-      <c r="B73" s="58"/>
+      <c r="B73" s="58" t="s">
+        <v>146</v>
+      </c>
       <c r="C73" s="59"/>
       <c r="D73" s="59"/>
       <c r="E73" s="59"/>
@@ -3573,135 +3686,105 @@
       <c r="K74" s="60"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A75" s="57"/>
-      <c r="B75" s="58" t="s">
+      <c r="A75" s="61" t="s">
         <v>148</v>
       </c>
-      <c r="C75" s="59"/>
-      <c r="D75" s="59"/>
-      <c r="E75" s="59"/>
-      <c r="F75" s="59"/>
-      <c r="G75" s="59"/>
-      <c r="H75" s="59"/>
-      <c r="I75" s="59"/>
-      <c r="J75" s="59"/>
-      <c r="K75" s="60"/>
+      <c r="B75" s="62"/>
+      <c r="C75" s="63"/>
+      <c r="D75" s="63"/>
+      <c r="E75" s="63"/>
+      <c r="F75" s="63"/>
+      <c r="G75" s="63"/>
+      <c r="H75" s="63"/>
+      <c r="I75" s="63"/>
+      <c r="J75" s="63"/>
+      <c r="K75" s="24"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A76" s="61" t="s">
+      <c r="A76" s="57"/>
+      <c r="B76" s="58"/>
+      <c r="C76" s="59"/>
+      <c r="D76" s="59"/>
+      <c r="E76" s="59"/>
+      <c r="F76" s="59"/>
+      <c r="G76" s="59"/>
+      <c r="H76" s="59"/>
+      <c r="I76" s="59"/>
+      <c r="J76" s="59"/>
+      <c r="K76" s="60"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A77" s="61" t="s">
         <v>149</v>
       </c>
-      <c r="B76" s="62"/>
-      <c r="C76" s="63"/>
-      <c r="D76" s="63"/>
-      <c r="E76" s="63"/>
-      <c r="F76" s="63"/>
-      <c r="G76" s="63"/>
-      <c r="H76" s="63"/>
-      <c r="I76" s="63"/>
-      <c r="J76" s="63"/>
-      <c r="K76" s="24"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A77" s="57"/>
-      <c r="B77" s="58"/>
-      <c r="C77" s="59"/>
-      <c r="D77" s="59"/>
-      <c r="E77" s="59"/>
-      <c r="F77" s="59"/>
-      <c r="G77" s="59"/>
-      <c r="H77" s="59"/>
-      <c r="I77" s="59"/>
-      <c r="J77" s="59"/>
-      <c r="K77" s="60"/>
+      <c r="B77" s="62"/>
+      <c r="C77" s="63"/>
+      <c r="D77" s="63"/>
+      <c r="E77" s="63"/>
+      <c r="F77" s="63"/>
+      <c r="G77" s="63"/>
+      <c r="H77" s="63"/>
+      <c r="I77" s="63"/>
+      <c r="J77" s="63"/>
+      <c r="K77" s="24"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A78" s="61" t="s">
+      <c r="A78" s="64"/>
+      <c r="B78" s="65"/>
+      <c r="C78" s="66"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="66"/>
+      <c r="F78" s="66"/>
+      <c r="G78" s="66"/>
+      <c r="H78" s="66"/>
+      <c r="I78" s="66"/>
+      <c r="J78" s="66"/>
+      <c r="K78" s="67"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A80" s="68" t="s">
         <v>150</v>
       </c>
-      <c r="B78" s="62"/>
-      <c r="C78" s="63"/>
-      <c r="D78" s="63"/>
-      <c r="E78" s="63"/>
-      <c r="F78" s="63"/>
-      <c r="G78" s="63"/>
-      <c r="H78" s="63"/>
-      <c r="I78" s="63"/>
-      <c r="J78" s="63"/>
-      <c r="K78" s="24"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A79" s="64"/>
-      <c r="B79" s="65"/>
-      <c r="C79" s="66"/>
-      <c r="D79" s="66"/>
-      <c r="E79" s="66"/>
-      <c r="F79" s="66"/>
-      <c r="G79" s="66"/>
-      <c r="H79" s="66"/>
-      <c r="I79" s="66"/>
-      <c r="J79" s="66"/>
-      <c r="K79" s="67"/>
+      <c r="B80" s="69"/>
+      <c r="C80" s="69"/>
+      <c r="D80" s="69"/>
+      <c r="E80" s="69"/>
+      <c r="F80" s="69"/>
+      <c r="G80" s="69"/>
+      <c r="H80" s="69"/>
+      <c r="I80" s="69"/>
+      <c r="J80" s="69"/>
+      <c r="K80" s="70"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A81" s="68" t="s">
+      <c r="A81" s="72" t="s">
         <v>151</v>
       </c>
-      <c r="B81" s="69"/>
-      <c r="C81" s="69"/>
-      <c r="D81" s="69"/>
-      <c r="E81" s="69"/>
-      <c r="F81" s="69"/>
-      <c r="G81" s="69"/>
-      <c r="H81" s="69"/>
-      <c r="I81" s="69"/>
-      <c r="J81" s="69"/>
-      <c r="K81" s="70"/>
+      <c r="B81" s="71"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="71"/>
+      <c r="E81" s="71"/>
+      <c r="F81" s="71"/>
+      <c r="G81" s="71"/>
+      <c r="H81" s="71"/>
+      <c r="I81" s="71"/>
+      <c r="J81" s="71"/>
+      <c r="K81" s="24"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A82" s="71" t="s">
+      <c r="A82" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="B82" s="72"/>
-      <c r="C82" s="72"/>
-      <c r="D82" s="72"/>
-      <c r="E82" s="72"/>
-      <c r="F82" s="72"/>
-      <c r="G82" s="72"/>
-      <c r="H82" s="72"/>
-      <c r="I82" s="72"/>
-      <c r="J82" s="72"/>
+      <c r="B82" s="71"/>
+      <c r="C82" s="71"/>
+      <c r="D82" s="71"/>
+      <c r="E82" s="71"/>
+      <c r="F82" s="71"/>
+      <c r="G82" s="71"/>
+      <c r="H82" s="71"/>
+      <c r="I82" s="71"/>
+      <c r="J82" s="71"/>
       <c r="K82" s="24"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A83" s="73" t="s">
-        <v>153</v>
-      </c>
-      <c r="B83" s="72"/>
-      <c r="C83" s="72"/>
-      <c r="D83" s="72"/>
-      <c r="E83" s="72"/>
-      <c r="F83" s="72"/>
-      <c r="G83" s="72"/>
-      <c r="H83" s="72"/>
-      <c r="I83" s="72"/>
-      <c r="J83" s="72"/>
-      <c r="K83" s="24"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A84" s="73" t="s">
-        <v>154</v>
-      </c>
-      <c r="B84" s="72"/>
-      <c r="C84" s="72"/>
-      <c r="D84" s="72"/>
-      <c r="E84" s="72"/>
-      <c r="F84" s="72"/>
-      <c r="G84" s="72"/>
-      <c r="H84" s="72"/>
-      <c r="I84" s="72"/>
-      <c r="J84" s="72"/>
-      <c r="K84" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
modification sur le readme
</commit_message>
<xml_diff>
--- a/docs/audit/audit-SEO.xlsx
+++ b/docs/audit/audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amama\Desktop\my projects\MahirAbubakar_P4_270621\docs\audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AAF1E6-BB91-4DD0-8246-ABCD69BD72A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AFCA3A-C747-4F13-A46B-BD6ACDE6D3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="157">
   <si>
     <t>Catégorie</t>
   </si>
@@ -341,34 +341,10 @@
     </r>
   </si>
   <si>
-    <t>Contexte</t>
-  </si>
-  <si>
-    <t>Site "vitrine" de l'agence de WebDesign "La Chouette Agence"</t>
-  </si>
-  <si>
-    <t>Rôle purement marketing : il s'agit de faire connaître l'agence, son offre, puis d'amener les visiteurs à cliquer sur la page "contactez nous", puis à remplir le formulaire</t>
-  </si>
-  <si>
     <t>Outils utilisés</t>
   </si>
   <si>
     <t>W3C Html&amp;Css</t>
-  </si>
-  <si>
-    <t>Test de vitesse sur Gtmetrix</t>
-  </si>
-  <si>
-    <t>Test de contenu dupliqué Siteliner</t>
-  </si>
-  <si>
-    <t>Test des mots clés avec Alize.info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Tanaguru </t>
-  </si>
-  <si>
-    <t>Outliner HTML5</t>
   </si>
   <si>
     <t>1. Detecter les problèmes</t>
@@ -535,6 +511,18 @@
   </si>
   <si>
     <t>Remove the empty link or provide text within the link that describes the functionality and/or target of that link.</t>
+  </si>
+  <si>
+    <t>LightHouse</t>
+  </si>
+  <si>
+    <t>Wave</t>
+  </si>
+  <si>
+    <t>Web Dev</t>
+  </si>
+  <si>
+    <t>WebAIM</t>
   </si>
 </sst>
 </file>
@@ -982,6 +970,15 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -990,15 +987,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1283,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z950"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="E1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1374,7 +1362,7 @@
       <c r="E3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="79" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1792,46 +1780,49 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="80" t="s">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="78" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="80" t="s">
+      <c r="B26" s="75" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="79" t="s">
-        <v>154</v>
-      </c>
-      <c r="C27" s="78" t="s">
-        <v>154</v>
-      </c>
-      <c r="D27" s="76" t="s">
-        <v>155</v>
-      </c>
-      <c r="E27" s="77" t="s">
-        <v>156</v>
+      <c r="B27" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="75" t="s">
+        <v>146</v>
+      </c>
+      <c r="D27" s="73" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="74" t="s">
+        <v>148</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B28" s="81" t="s">
-        <v>157</v>
-      </c>
-      <c r="C28" s="78" t="s">
-        <v>158</v>
-      </c>
-      <c r="D28" s="78" t="s">
-        <v>159</v>
-      </c>
-      <c r="E28" s="78" t="s">
-        <v>160</v>
+      <c r="A28" s="77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="78" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="D28" s="75" t="s">
+        <v>151</v>
+      </c>
+      <c r="E28" s="75" t="s">
+        <v>152</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>30</v>
@@ -2794,10 +2785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE5A153-4088-4B3A-B952-ECA3228BDD93}">
-  <dimension ref="A1:K82"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N63" sqref="N63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2807,17 +2798,17 @@
     <col min="11" max="11" width="5.921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E1" s="73" t="s">
+    <row r="1" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E1" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="75"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>98</v>
       </c>
@@ -2825,10 +2816,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="15"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>100</v>
       </c>
@@ -2836,69 +2827,98 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14"/>
       <c r="B8" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="15"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="19"/>
+      <c r="B17" s="25" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="18"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="21"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
@@ -2910,38 +2930,38 @@
       <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="24"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="19"/>
-      <c r="B20" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="21"/>
+      <c r="A20" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="20"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="25" t="s">
+        <v>106</v>
+      </c>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -2967,7 +2987,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
@@ -2983,7 +3003,7 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="19"/>
       <c r="B24" s="25" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
@@ -2996,8 +3016,10 @@
       <c r="K24" s="21"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="20"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="26" t="s">
+        <v>109</v>
+      </c>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -3009,25 +3031,23 @@
       <c r="K25" s="21"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="24"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="19"/>
-      <c r="B27" s="25" t="s">
-        <v>116</v>
-      </c>
+      <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
@@ -3039,24 +3059,24 @@
       <c r="K27" s="21"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="19"/>
-      <c r="B28" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="21"/>
+      <c r="A28" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="24"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="19"/>
-      <c r="B29" s="26" t="s">
-        <v>118</v>
+      <c r="B29" s="25" t="s">
+        <v>112</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
@@ -3069,78 +3089,78 @@
       <c r="K29" s="21"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="19"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="21"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="24"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="29"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="19"/>
-      <c r="B32" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="21"/>
+      <c r="A32" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="32"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="27"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="29"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="35"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="24"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="32"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="35"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="33"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="34"/>
       <c r="C36" s="34"/>
       <c r="D36" s="34"/>
@@ -3154,7 +3174,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="36" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B37" s="37"/>
       <c r="C37" s="37"/>
@@ -3169,9 +3189,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="34"/>
-      <c r="B38" s="38" t="s">
-        <v>123</v>
-      </c>
+      <c r="B38" s="34"/>
       <c r="C38" s="34"/>
       <c r="D38" s="34"/>
       <c r="E38" s="34"/>
@@ -3183,64 +3201,66 @@
       <c r="K38" s="35"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="35"/>
+      <c r="A39" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="24"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="24"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="35"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="34"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="34"/>
-      <c r="K41" s="35"/>
+      <c r="A41" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="24"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="24"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
+      <c r="K42" s="35"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
+      <c r="B43" s="38"/>
       <c r="C43" s="34"/>
       <c r="D43" s="34"/>
       <c r="E43" s="34"/>
@@ -3253,7 +3273,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="36" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B44" s="37"/>
       <c r="C44" s="37"/>
@@ -3268,9 +3288,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="34"/>
-      <c r="B45" s="39" t="s">
-        <v>127</v>
-      </c>
+      <c r="B45" s="34"/>
       <c r="C45" s="34"/>
       <c r="D45" s="34"/>
       <c r="E45" s="34"/>
@@ -3282,36 +3300,40 @@
       <c r="K45" s="35"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" s="34"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="35"/>
+      <c r="A46" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="24"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="24"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="35"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="34"/>
-      <c r="B48" s="34"/>
+      <c r="B48" s="39" t="s">
+        <v>123</v>
+      </c>
       <c r="C48" s="34"/>
       <c r="D48" s="34"/>
       <c r="E48" s="34"/>
@@ -3323,10 +3345,10 @@
       <c r="K48" s="35"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="B49" s="37"/>
+      <c r="A49" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" s="41"/>
       <c r="C49" s="37"/>
       <c r="D49" s="37"/>
       <c r="E49" s="37"/>
@@ -3338,9 +3360,9 @@
       <c r="K49" s="24"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A50" s="34"/>
+      <c r="A50" s="42"/>
       <c r="B50" s="39" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C50" s="34"/>
       <c r="D50" s="34"/>
@@ -3353,9 +3375,9 @@
       <c r="K50" s="35"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A51" s="34"/>
+      <c r="A51" s="42"/>
       <c r="B51" s="39" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C51" s="34"/>
       <c r="D51" s="34"/>
@@ -3368,39 +3390,37 @@
       <c r="K51" s="35"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="B52" s="41"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="37"/>
-      <c r="J52" s="37"/>
-      <c r="K52" s="24"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="34"/>
+      <c r="K52" s="35"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A53" s="42"/>
-      <c r="B53" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="34"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="34"/>
-      <c r="K53" s="35"/>
+      <c r="A53" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="24"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A54" s="42"/>
-      <c r="B54" s="39" t="s">
-        <v>134</v>
+      <c r="A54" s="34"/>
+      <c r="B54" s="38" t="s">
+        <v>128</v>
       </c>
       <c r="C54" s="34"/>
       <c r="D54" s="34"/>
@@ -3414,7 +3434,9 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="34"/>
-      <c r="B55" s="39"/>
+      <c r="B55" s="38" t="s">
+        <v>129</v>
+      </c>
       <c r="C55" s="34"/>
       <c r="D55" s="34"/>
       <c r="E55" s="34"/>
@@ -3426,25 +3448,23 @@
       <c r="K55" s="35"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A56" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="B56" s="37"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="37"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="24"/>
+      <c r="A56" s="34"/>
+      <c r="B56" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="34"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="34"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="34"/>
+      <c r="J56" s="34"/>
+      <c r="K56" s="35"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="34"/>
-      <c r="B57" s="38" t="s">
-        <v>136</v>
-      </c>
+      <c r="B57" s="38"/>
       <c r="C57" s="34"/>
       <c r="D57" s="34"/>
       <c r="E57" s="34"/>
@@ -3456,38 +3476,38 @@
       <c r="K57" s="35"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A58" s="34"/>
-      <c r="B58" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="34"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="34"/>
-      <c r="K58" s="35"/>
+      <c r="A58" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="24"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A59" s="34"/>
-      <c r="B59" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="34"/>
-      <c r="K59" s="35"/>
+      <c r="A59" s="44"/>
+      <c r="B59" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="31"/>
+      <c r="K59" s="32"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A60" s="34"/>
-      <c r="B60" s="38"/>
+      <c r="A60" s="46"/>
+      <c r="B60" s="39"/>
       <c r="C60" s="34"/>
       <c r="D60" s="34"/>
       <c r="E60" s="34"/>
@@ -3499,95 +3519,95 @@
       <c r="K60" s="35"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A61" s="43" t="s">
-        <v>139</v>
-      </c>
-      <c r="B61" s="37"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="37"/>
-      <c r="J61" s="37"/>
+      <c r="A61" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="B61" s="48"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="49"/>
+      <c r="J61" s="49"/>
       <c r="K61" s="24"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A62" s="44"/>
-      <c r="B62" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="C62" s="31"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="31"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31"/>
-      <c r="H62" s="31"/>
-      <c r="I62" s="31"/>
-      <c r="J62" s="31"/>
-      <c r="K62" s="32"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A63" s="46"/>
-      <c r="B63" s="39"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="34"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="35"/>
+      <c r="A62" s="50"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="52"/>
+      <c r="F62" s="52"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="53"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A64" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="B64" s="48"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="49"/>
-      <c r="E64" s="49"/>
-      <c r="F64" s="49"/>
-      <c r="G64" s="49"/>
-      <c r="H64" s="49"/>
-      <c r="I64" s="49"/>
-      <c r="J64" s="49"/>
-      <c r="K64" s="24"/>
+      <c r="A64" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" s="55"/>
+      <c r="C64" s="55"/>
+      <c r="D64" s="55"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="55"/>
+      <c r="G64" s="55"/>
+      <c r="H64" s="55"/>
+      <c r="I64" s="55"/>
+      <c r="J64" s="55"/>
+      <c r="K64" s="56"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A65" s="50"/>
-      <c r="B65" s="51"/>
-      <c r="C65" s="52"/>
-      <c r="D65" s="52"/>
-      <c r="E65" s="52"/>
-      <c r="F65" s="52"/>
-      <c r="G65" s="52"/>
-      <c r="H65" s="52"/>
-      <c r="I65" s="52"/>
-      <c r="J65" s="52"/>
-      <c r="K65" s="53"/>
+      <c r="A65" s="57"/>
+      <c r="B65" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="59"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="59"/>
+      <c r="F65" s="59"/>
+      <c r="G65" s="59"/>
+      <c r="H65" s="59"/>
+      <c r="I65" s="59"/>
+      <c r="J65" s="59"/>
+      <c r="K65" s="60"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A66" s="57"/>
+      <c r="B66" s="58"/>
+      <c r="C66" s="59"/>
+      <c r="D66" s="59"/>
+      <c r="E66" s="59"/>
+      <c r="F66" s="59"/>
+      <c r="G66" s="59"/>
+      <c r="H66" s="59"/>
+      <c r="I66" s="59"/>
+      <c r="J66" s="59"/>
+      <c r="K66" s="60"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A67" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="B67" s="55"/>
-      <c r="C67" s="55"/>
-      <c r="D67" s="55"/>
-      <c r="E67" s="55"/>
-      <c r="F67" s="55"/>
-      <c r="G67" s="55"/>
-      <c r="H67" s="55"/>
-      <c r="I67" s="55"/>
-      <c r="J67" s="55"/>
-      <c r="K67" s="56"/>
+      <c r="A67" s="57"/>
+      <c r="B67" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" s="59"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="59"/>
+      <c r="F67" s="59"/>
+      <c r="G67" s="59"/>
+      <c r="H67" s="59"/>
+      <c r="I67" s="59"/>
+      <c r="J67" s="59"/>
+      <c r="K67" s="60"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="57"/>
       <c r="B68" s="58" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C68" s="59"/>
       <c r="D68" s="59"/>
@@ -3615,7 +3635,7 @@
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="57"/>
       <c r="B70" s="58" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C70" s="59"/>
       <c r="D70" s="59"/>
@@ -3630,7 +3650,7 @@
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="57"/>
       <c r="B71" s="58" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C71" s="59"/>
       <c r="D71" s="59"/>
@@ -3643,23 +3663,23 @@
       <c r="K71" s="60"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A72" s="57"/>
-      <c r="B72" s="58"/>
-      <c r="C72" s="59"/>
-      <c r="D72" s="59"/>
-      <c r="E72" s="59"/>
-      <c r="F72" s="59"/>
-      <c r="G72" s="59"/>
-      <c r="H72" s="59"/>
-      <c r="I72" s="59"/>
-      <c r="J72" s="59"/>
-      <c r="K72" s="60"/>
+      <c r="A72" s="61" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" s="62"/>
+      <c r="C72" s="63"/>
+      <c r="D72" s="63"/>
+      <c r="E72" s="63"/>
+      <c r="F72" s="63"/>
+      <c r="G72" s="63"/>
+      <c r="H72" s="63"/>
+      <c r="I72" s="63"/>
+      <c r="J72" s="63"/>
+      <c r="K72" s="24"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="57"/>
-      <c r="B73" s="58" t="s">
-        <v>146</v>
-      </c>
+      <c r="B73" s="58"/>
       <c r="C73" s="59"/>
       <c r="D73" s="59"/>
       <c r="E73" s="59"/>
@@ -3671,120 +3691,77 @@
       <c r="K73" s="60"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A74" s="57"/>
-      <c r="B74" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="C74" s="59"/>
-      <c r="D74" s="59"/>
-      <c r="E74" s="59"/>
-      <c r="F74" s="59"/>
-      <c r="G74" s="59"/>
-      <c r="H74" s="59"/>
-      <c r="I74" s="59"/>
-      <c r="J74" s="59"/>
-      <c r="K74" s="60"/>
+      <c r="A74" s="61" t="s">
+        <v>141</v>
+      </c>
+      <c r="B74" s="62"/>
+      <c r="C74" s="63"/>
+      <c r="D74" s="63"/>
+      <c r="E74" s="63"/>
+      <c r="F74" s="63"/>
+      <c r="G74" s="63"/>
+      <c r="H74" s="63"/>
+      <c r="I74" s="63"/>
+      <c r="J74" s="63"/>
+      <c r="K74" s="24"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A75" s="61" t="s">
-        <v>148</v>
-      </c>
-      <c r="B75" s="62"/>
-      <c r="C75" s="63"/>
-      <c r="D75" s="63"/>
-      <c r="E75" s="63"/>
-      <c r="F75" s="63"/>
-      <c r="G75" s="63"/>
-      <c r="H75" s="63"/>
-      <c r="I75" s="63"/>
-      <c r="J75" s="63"/>
-      <c r="K75" s="24"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A76" s="57"/>
-      <c r="B76" s="58"/>
-      <c r="C76" s="59"/>
-      <c r="D76" s="59"/>
-      <c r="E76" s="59"/>
-      <c r="F76" s="59"/>
-      <c r="G76" s="59"/>
-      <c r="H76" s="59"/>
-      <c r="I76" s="59"/>
-      <c r="J76" s="59"/>
-      <c r="K76" s="60"/>
+      <c r="A75" s="64"/>
+      <c r="B75" s="65"/>
+      <c r="C75" s="66"/>
+      <c r="D75" s="66"/>
+      <c r="E75" s="66"/>
+      <c r="F75" s="66"/>
+      <c r="G75" s="66"/>
+      <c r="H75" s="66"/>
+      <c r="I75" s="66"/>
+      <c r="J75" s="66"/>
+      <c r="K75" s="67"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A77" s="61" t="s">
-        <v>149</v>
-      </c>
-      <c r="B77" s="62"/>
-      <c r="C77" s="63"/>
-      <c r="D77" s="63"/>
-      <c r="E77" s="63"/>
-      <c r="F77" s="63"/>
-      <c r="G77" s="63"/>
-      <c r="H77" s="63"/>
-      <c r="I77" s="63"/>
-      <c r="J77" s="63"/>
-      <c r="K77" s="24"/>
+      <c r="A77" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="B77" s="69"/>
+      <c r="C77" s="69"/>
+      <c r="D77" s="69"/>
+      <c r="E77" s="69"/>
+      <c r="F77" s="69"/>
+      <c r="G77" s="69"/>
+      <c r="H77" s="69"/>
+      <c r="I77" s="69"/>
+      <c r="J77" s="69"/>
+      <c r="K77" s="70"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A78" s="64"/>
-      <c r="B78" s="65"/>
-      <c r="C78" s="66"/>
-      <c r="D78" s="66"/>
-      <c r="E78" s="66"/>
-      <c r="F78" s="66"/>
-      <c r="G78" s="66"/>
-      <c r="H78" s="66"/>
-      <c r="I78" s="66"/>
-      <c r="J78" s="66"/>
-      <c r="K78" s="67"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A80" s="68" t="s">
-        <v>150</v>
-      </c>
-      <c r="B80" s="69"/>
-      <c r="C80" s="69"/>
-      <c r="D80" s="69"/>
-      <c r="E80" s="69"/>
-      <c r="F80" s="69"/>
-      <c r="G80" s="69"/>
-      <c r="H80" s="69"/>
-      <c r="I80" s="69"/>
-      <c r="J80" s="69"/>
-      <c r="K80" s="70"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A81" s="72" t="s">
-        <v>151</v>
-      </c>
-      <c r="B81" s="71"/>
-      <c r="C81" s="71"/>
-      <c r="D81" s="71"/>
-      <c r="E81" s="71"/>
-      <c r="F81" s="71"/>
-      <c r="G81" s="71"/>
-      <c r="H81" s="71"/>
-      <c r="I81" s="71"/>
-      <c r="J81" s="71"/>
-      <c r="K81" s="24"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A82" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="B82" s="71"/>
-      <c r="C82" s="71"/>
-      <c r="D82" s="71"/>
-      <c r="E82" s="71"/>
-      <c r="F82" s="71"/>
-      <c r="G82" s="71"/>
-      <c r="H82" s="71"/>
-      <c r="I82" s="71"/>
-      <c r="J82" s="71"/>
-      <c r="K82" s="24"/>
+      <c r="A78" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="B78" s="71"/>
+      <c r="C78" s="71"/>
+      <c r="D78" s="71"/>
+      <c r="E78" s="71"/>
+      <c r="F78" s="71"/>
+      <c r="G78" s="71"/>
+      <c r="H78" s="71"/>
+      <c r="I78" s="71"/>
+      <c r="J78" s="71"/>
+      <c r="K78" s="24"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A79" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="B79" s="71"/>
+      <c r="C79" s="71"/>
+      <c r="D79" s="71"/>
+      <c r="E79" s="71"/>
+      <c r="F79" s="71"/>
+      <c r="G79" s="71"/>
+      <c r="H79" s="71"/>
+      <c r="I79" s="71"/>
+      <c r="J79" s="71"/>
+      <c r="K79" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>